<commit_message>
Table Created in XLSX.
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A5:C12"/>
+  <dimension ref="A5:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,11 +430,21 @@
           <t>Diary No</t>
         </is>
       </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>Diary No.- 1 - 2020</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Who Vs Who</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>MANISHA BISHT vs. VIKAS KANWAR</t>
         </is>
       </c>
     </row>
@@ -450,11 +460,128 @@
     <row r="10"/>
     <row r="11"/>
     <row r="12"/>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Diary No</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>Diary No.- 2 - 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Who Vs Who</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>CITY MONTESSORI SCHOOL vs. ASHOK BHARGAVA</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Case Details</t>
+        </is>
+      </c>
+    </row>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Diary No</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>Diary No.- 1 - 2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Who Vs Who</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>C. KALIDAS vs. THE SECRETARY TAMIL NADU PUBLIC SERVICE COMMISSION</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>Case Details</t>
+        </is>
+      </c>
+    </row>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>Diary No</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>Diary No.- 2 - 2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>Who Vs Who</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>P. SATISH KUMAR vs. UNION OF INDIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>Case Details</t>
+        </is>
+      </c>
+    </row>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="12">
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="A7:A12"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="A37:A42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>